<commit_message>
Updated to do list
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="0" windowWidth="10785" windowHeight="2558" activeTab="1"/>
+    <workbookView xWindow="2970" yWindow="0" windowWidth="10785" windowHeight="2558"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
-  <si>
-    <t>Github: https://github.com/ruohanliu/Gdax/</t>
-  </si>
-  <si>
-    <t>Api: https://docs.gdax.com/</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -94,7 +88,94 @@
     <t>facilitate implementing model</t>
   </si>
   <si>
-    <t>Compute a variaty of indices, such as RSI</t>
+    <t>http://wiki.mbalib.com/wiki/%E8%83%BD%E9%87%8F%E6%BD%AE%E6%8C%87%E6%A0%87</t>
+  </si>
+  <si>
+    <t>OBV</t>
+  </si>
+  <si>
+    <t>Api</t>
+  </si>
+  <si>
+    <t>https://docs.gdax.com/</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>https://github.com/ruohanliu/Gdax/</t>
+  </si>
+  <si>
+    <t>RSI</t>
+  </si>
+  <si>
+    <t>https://zh.wikipedia.org/wiki/%E7%9B%B8%E5%B0%8D%E5%BC%B7%E5%BC%B1%E6%8C%87%E6%95%B8</t>
+  </si>
+  <si>
+    <t>http://www.investopedia.com/terms/o/onbalancevolume.asp</t>
+  </si>
+  <si>
+    <t>more indices</t>
+  </si>
+  <si>
+    <t>https://www.interactivebrokers.co.jp/cn/index.php?f=13549</t>
+  </si>
+  <si>
+    <t>TSI</t>
+  </si>
+  <si>
+    <t>https://tradingsim.com/blog/true-strength-index/</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Relative_strength_index</t>
+  </si>
+  <si>
+    <t>MACD</t>
+  </si>
+  <si>
+    <t>https://zh.wikipedia.org/wiki/MACD</t>
+  </si>
+  <si>
+    <t>Dictionary:interval_book
+key:interval_start_time
+value: (Bid_Price_Index,Ask_Price_Index)</t>
+  </si>
+  <si>
+    <t>Compute a variaty of indices</t>
+  </si>
+  <si>
+    <t>MACD
+Volume EMA
+RSI
+TSI
+OBV</t>
+  </si>
+  <si>
+    <t>Current using intervals: 1s, 30s, 120s</t>
+  </si>
+  <si>
+    <t>Test Private API using sandbox</t>
+  </si>
+  <si>
+    <t>Test Private API on Gdax</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>Complete the necessary functions</t>
+  </si>
+  <si>
+    <t>To be safe</t>
+  </si>
+  <si>
+    <t>Volume EMA</t>
+  </si>
+  <si>
+    <t>How to use?
+Useful?
+Time needed to take effect?
+How to normalize?</t>
   </si>
 </sst>
 </file>
@@ -461,25 +542,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.73046875" customWidth="1"/>
+    <col min="1" max="1" width="13.59765625" customWidth="1"/>
+    <col min="2" max="2" width="53.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -491,7 +625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -501,64 +637,78 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
@@ -710,9 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -722,64 +870,76 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
@@ -930,9 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -942,52 +1100,72 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="58.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1144,19 +1322,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>